<commit_message>
added tests for ifce robot manipulator
</commit_message>
<xml_diff>
--- a/results_analysis/knn-sparse_motor_failure/Knn Sparse - Mot Fail - Resumo.xlsx
+++ b/results_analysis/knn-sparse_motor_failure/Knn Sparse - Mot Fail - Resumo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results\knn-sparse_motor_failure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\knn-sparse_motor_failure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DB7A78-0588-4F37-86AE-52400F28F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E0A89-A716-4B8B-8D1E-232F30FFBD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,79 +399,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -757,12 +754,12 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
@@ -775,19 +772,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -800,28 +797,28 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -835,123 +832,122 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>70</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>73</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>72</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>85</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>89</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="10">
         <v>50</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>63</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="24">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <v>63</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>80</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>78</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>87</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>89</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>50</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>85</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="15">
         <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="14">
         <v>71</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>80</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>78</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>87</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>89</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>50</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>72</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="15">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>33</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>81</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="17">
         <v>28</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="18">
         <v>89</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="18">
         <v>83</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="17">
         <v>50</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>68</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="19">
         <v>87</v>
       </c>
     </row>
@@ -965,123 +961,122 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <v>80</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>75</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>87</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>89</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="13">
         <v>91</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <v>50</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <v>81</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="20">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>79</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>87</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>78</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>89</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>93</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <v>50</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="8">
         <v>73</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="21">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="5">
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>82</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>73</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>78</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>85</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>90</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="8">
         <v>55</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="8">
         <v>75</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="21">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>78</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="17">
         <v>82</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="17">
         <v>73</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <v>85</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="18">
         <v>91</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="17">
         <v>52</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="17">
         <v>78</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="22">
         <v>89</v>
       </c>
     </row>
@@ -1095,123 +1090,122 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>90</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>80</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>85</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="13">
         <v>90</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>85</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="13">
         <v>90</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="12">
         <v>82</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="20">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="14">
         <v>90</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>89</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>83</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>92</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>91</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="7">
         <v>90</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <v>75</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="21">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="5">
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="14">
         <v>60</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>55</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <v>52</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="8">
         <v>55</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="8">
         <v>52</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>58</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <v>51</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="15">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>48</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="17">
         <v>52</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="17">
         <v>62</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="17">
         <v>53</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="17">
         <v>54</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="17">
         <v>52</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="17">
         <v>55</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="19">
         <v>52</v>
       </c>
     </row>
@@ -1219,129 +1213,128 @@
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <v>91</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>91</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="12">
         <v>73</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="13">
         <v>91</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="13">
         <v>91</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="12">
         <v>52</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="12">
         <v>79</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="20">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="14">
         <v>91</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>91</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <v>79</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>91</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <v>91</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>50</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>68</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="21">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="5">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="14">
         <v>72</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <v>73</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="8">
         <v>78</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>80</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>82</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>60</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <v>72</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="21">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>71</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>73</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="17">
         <v>78</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="18">
         <v>91</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="18">
         <v>92</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="17">
         <v>53</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="17">
         <v>68</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="22">
         <v>83</v>
       </c>
     </row>

</xml_diff>